<commit_message>
WIP commit - refactoring UI
</commit_message>
<xml_diff>
--- a/docs/EasyFPUViewStructure.xlsx
+++ b/docs/EasyFPUViewStructure.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ulrich/Repositories/iOS-EasyFPU/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{358BAE90-96DF-A749-ACB2-E9C4E5FF9074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5D1BA7B-6407-9049-881E-CF1419C7A8F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="49820" yWindow="6520" windowWidth="28240" windowHeight="17240" xr2:uid="{69B919E2-0FE3-844B-BBA9-A58DA31614E3}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{69B919E2-0FE3-844B-BBA9-A58DA31614E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="ID management" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>MainView</t>
   </si>
@@ -69,6 +70,33 @@
   </si>
   <si>
     <t>HelpView</t>
+  </si>
+  <si>
+    <t>new</t>
+  </si>
+  <si>
+    <t>new Ingredient</t>
+  </si>
+  <si>
+    <t>FoodItem.id</t>
+  </si>
+  <si>
+    <t>then id =</t>
+  </si>
+  <si>
+    <t>When</t>
+  </si>
+  <si>
+    <t>new ComposedFoodItem</t>
+  </si>
+  <si>
+    <t>FoodItem from FoodItemVM</t>
+  </si>
+  <si>
+    <t>FoodItemVM.id</t>
+  </si>
+  <si>
+    <t>FoodItem from ComposedFoodItemVM</t>
   </si>
 </sst>
 </file>
@@ -445,7 +473,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{997533CC-42B0-1C4B-8A0A-33AA353A1C3A}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -519,4 +547,62 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38A299DD-9CBA-8649-8E59-34AEC673CBB2}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="32.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>